<commit_message>
update report and chiller overwrite scenarios
</commit_message>
<xml_diff>
--- a/MMA_Merchandising/MMA_Merchandising.xlsx
+++ b/MMA_Merchandising/MMA_Merchandising.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D2B1E-DB8B-414F-948B-57074E8E2B07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC40A84-EF00-4648-BAB0-AAEAC8CC3473}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="3" activeTab="5" xr2:uid="{65B03DFA-846A-4EE9-BFD9-C2885113F2BF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="1" xr2:uid="{65B03DFA-846A-4EE9-BFD9-C2885113F2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution Point" sheetId="11" r:id="rId1"/>
@@ -1442,9 +1442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE23399-18E8-4586-AB6F-57ACC320652C}">
   <dimension ref="A1:T1634"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1546" sqref="B1546"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1637" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1646" sqref="D1646"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6025,7 +6025,7 @@
         <v>19</v>
       </c>
       <c r="C120" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D120" t="s">
         <v>192</v>
@@ -6063,7 +6063,7 @@
         <v>19</v>
       </c>
       <c r="C121" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D121" t="s">
         <v>193</v>
@@ -8419,7 +8419,7 @@
         <v>19</v>
       </c>
       <c r="C183" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D183" t="s">
         <v>192</v>
@@ -8457,7 +8457,7 @@
         <v>19</v>
       </c>
       <c r="C184" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D184" t="s">
         <v>193</v>
@@ -14347,7 +14347,7 @@
         <v>19</v>
       </c>
       <c r="C339" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D339" t="s">
         <v>192</v>
@@ -14385,7 +14385,7 @@
         <v>19</v>
       </c>
       <c r="C340" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D340" t="s">
         <v>193</v>
@@ -18793,7 +18793,7 @@
         <v>19</v>
       </c>
       <c r="C456" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D456" t="s">
         <v>192</v>
@@ -18831,7 +18831,7 @@
         <v>19</v>
       </c>
       <c r="C457" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D457" t="s">
         <v>193</v>
@@ -23505,7 +23505,7 @@
         <v>19</v>
       </c>
       <c r="C580" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D580" t="s">
         <v>192</v>
@@ -23543,7 +23543,7 @@
         <v>19</v>
       </c>
       <c r="C581" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D581" t="s">
         <v>193</v>
@@ -30877,7 +30877,7 @@
         <v>19</v>
       </c>
       <c r="C774" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D774" t="s">
         <v>192</v>
@@ -30915,7 +30915,7 @@
         <v>19</v>
       </c>
       <c r="C775" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D775" t="s">
         <v>193</v>
@@ -34373,7 +34373,7 @@
         <v>19</v>
       </c>
       <c r="C866" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D866" t="s">
         <v>192</v>
@@ -34411,7 +34411,7 @@
         <v>19</v>
       </c>
       <c r="C867" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D867" t="s">
         <v>193</v>
@@ -35969,7 +35969,7 @@
         <v>19</v>
       </c>
       <c r="C908" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D908" t="s">
         <v>192</v>
@@ -36007,7 +36007,7 @@
         <v>19</v>
       </c>
       <c r="C909" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D909" t="s">
         <v>193</v>
@@ -43531,7 +43531,7 @@
         <v>19</v>
       </c>
       <c r="C1107" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1107" t="s">
         <v>192</v>
@@ -43569,7 +43569,7 @@
         <v>19</v>
       </c>
       <c r="C1108" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1108" t="s">
         <v>193</v>
@@ -48129,7 +48129,7 @@
         <v>19</v>
       </c>
       <c r="C1228" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1228" t="s">
         <v>192</v>
@@ -48167,7 +48167,7 @@
         <v>19</v>
       </c>
       <c r="C1229" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1229" t="s">
         <v>193</v>
@@ -51131,7 +51131,7 @@
         <v>19</v>
       </c>
       <c r="C1307" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1307" t="s">
         <v>192</v>
@@ -51169,7 +51169,7 @@
         <v>19</v>
       </c>
       <c r="C1308" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1308" t="s">
         <v>193</v>
@@ -54931,7 +54931,7 @@
         <v>19</v>
       </c>
       <c r="C1407" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1407" t="s">
         <v>192</v>
@@ -54969,7 +54969,7 @@
         <v>19</v>
       </c>
       <c r="C1408" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1408" t="s">
         <v>193</v>
@@ -58389,7 +58389,7 @@
         <v>19</v>
       </c>
       <c r="C1498" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1498" t="s">
         <v>192</v>
@@ -58427,7 +58427,7 @@
         <v>19</v>
       </c>
       <c r="C1499" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1499" t="s">
         <v>193</v>
@@ -62607,7 +62607,7 @@
         <v>19</v>
       </c>
       <c r="C1609" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1609" t="s">
         <v>192</v>
@@ -62645,7 +62645,7 @@
         <v>19</v>
       </c>
       <c r="C1610" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="D1610" t="s">
         <v>193</v>
@@ -68350,7 +68350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F3C5A3-D5BE-4ACF-B6DB-094F3337EE5F}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>